<commit_message>
salary demo + attendance + generate attendance
</commit_message>
<xml_diff>
--- a/backend/uploads/ExtractedFiles/1247.xlsx
+++ b/backend/uploads/ExtractedFiles/1247.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14625"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="14630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -401,9 +399,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -449,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -472,7 +470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -495,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -518,7 +516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -541,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -564,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -587,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -610,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -633,7 +631,7 @@
         <v>9.1000003814697266</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -656,7 +654,7 @@
         <v>9.2399997711181641</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -679,7 +677,7 @@
         <v>9.119999885559082</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -702,7 +700,7 @@
         <v>9.1400003433227539</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -725,7 +723,7 @@
         <v>9.1099996566772461</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -748,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -771,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -794,7 +792,7 @@
         <v>9.1899995803833008</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -817,7 +815,7 @@
         <v>9.0900001525878906</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -840,7 +838,7 @@
         <v>9.2399997711181641</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -863,7 +861,7 @@
         <v>9.0900001525878906</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -886,7 +884,7 @@
         <v>9.2700004577636719</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -909,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -932,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -955,7 +953,7 @@
         <v>9.0500001907348633</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -978,7 +976,7 @@
         <v>6.5500001907348633</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1001,7 +999,7 @@
         <v>7.1700000762939453</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1022,7 @@
         <v>9.380000114440918</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1047,7 +1045,7 @@
         <v>9.5399999618530273</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1114,7 @@
         <v>9.5699996948242187</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1137,7 @@
         <v>10.090000152587891</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1162,7 +1160,7 @@
         <v>10.039999961853027</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1183,7 @@
         <v>9.1800003051757813</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1206,7 @@
         <v>9.2100000381469727</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1231,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1254,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1300,7 +1298,7 @@
         <v>9.5500001907348633</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1346,7 +1344,7 @@
         <v>9.119999885559082</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1367,7 @@
         <v>9.0600004196166992</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1392,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1415,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1436,7 @@
         <v>9.0900001525878906</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1459,7 @@
         <v>9.0799999237060547</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1482,7 @@
         <v>9.0299997329711914</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1505,7 @@
         <v>9.130000114440918</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1553,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1576,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1599,7 +1597,7 @@
         <v>9.130000114440918</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1622,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1645,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1668,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1691,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -1737,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1760,7 +1758,7 @@
         <v>9.1599998474121094</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1783,7 +1781,7 @@
         <v>9.1599998474121094</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1809,28 +1807,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>